<commit_message>
draft version of rules_to_pydantic_model
</commit_message>
<xml_diff>
--- a/cognite/neat/rules/examples/source-to-solution-mapping-rules.xlsx
+++ b/cognite/neat/rules/examples/source-to-solution-mapping-rules.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/cognite/neat/examples/rules/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/cognite/neat/rules/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61021A0-7F8D-DA42-A5A4-20BA568044BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73A3004-44B7-9D48-9ED7-88C32B3B33B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -1714,7 +1714,7 @@
   </sheetPr>
   <dimension ref="A1:W999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -27290,8 +27290,8 @@
   </sheetPr>
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView zoomScale="140" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -28072,9 +28072,7 @@
       <c r="D19" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="33">
-        <v>1</v>
-      </c>
+      <c r="E19" s="33"/>
       <c r="F19" s="33">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Feature gen construct query (#88)
- Generation of in-memory pydantic models based on class/property definitions in `TransformationRules`
- Generation of `CONSTRUCT` query which provides "views" into source graph and in most cases alleviate the need of creating solution graph
</commit_message>
<xml_diff>
--- a/cognite/neat/rules/examples/source-to-solution-mapping-rules.xlsx
+++ b/cognite/neat/rules/examples/source-to-solution-mapping-rules.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/cognite/neat/examples/rules/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/cognite/neat/rules/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61021A0-7F8D-DA42-A5A4-20BA568044BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73A3004-44B7-9D48-9ED7-88C32B3B33B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -1714,7 +1714,7 @@
   </sheetPr>
   <dimension ref="A1:W999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -27290,8 +27290,8 @@
   </sheetPr>
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView zoomScale="140" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -28072,9 +28072,7 @@
       <c r="D19" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="33">
-        <v>1</v>
-      </c>
+      <c r="E19" s="33"/>
       <c r="F19" s="33">
         <v>1</v>
       </c>

</xml_diff>